<commit_message>
Removed environment file and updated requirement.text
</commit_message>
<xml_diff>
--- a/data/Monthly Infographic - Hyperlinks.xlsx
+++ b/data/Monthly Infographic - Hyperlinks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ParikH01\OneDrive - CPGPLC\Desktop\infographic automation\Infographic-Automation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpgplc-my.sharepoint.com/personal/hard_parikh_compass-usa_com/Documents/Desktop/infographic automation/Infographic-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF37231-5EA1-41B8-9F7E-24F4E4A33F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="646" documentId="13_ncr:1_{3EF37231-5EA1-41B8-9F7E-24F4E4A33F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA679134-CD4C-427A-A7F5-EA597D886BEB}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>